<commit_message>
added makefile and updated README
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matanel\Documents\University\Year2\SemesterB\67808-OS\Exercises\Ex1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B24E52-C03E-4B00-8D7A-8B2495D3A0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E1F4AF-BA4A-49C3-860B-7125C7652CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30168" windowHeight="20184" xr2:uid="{C6A71BF6-A859-455F-B82C-36D33C55CA41}"/>
   </bookViews>
@@ -37,15 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
-    <t>Directry On Machine</t>
-  </si>
-  <si>
-    <t>On VM</t>
-  </si>
-  <si>
-    <t>On Container</t>
-  </si>
-  <si>
     <t>iterations = 100</t>
   </si>
   <si>
@@ -62,6 +53,15 @@
   </si>
   <si>
     <t>Trap</t>
+  </si>
+  <si>
+    <t>Directly On Machine</t>
+  </si>
+  <si>
+    <t>Using a Container</t>
+  </si>
+  <si>
+    <t>Using a VM</t>
   </si>
 </sst>
 </file>
@@ -209,7 +209,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Directry On Machine</c:v>
+                  <c:v>Directly On Machine</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -274,7 +274,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On Container</c:v>
+                  <c:v>Using a Container</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -339,7 +339,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On VM</c:v>
+                  <c:v>Using a VM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -684,7 +684,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Directry On Machine</c:v>
+                  <c:v>Directly On Machine</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -749,7 +749,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On Container</c:v>
+                  <c:v>Using a Container</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -814,7 +814,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On VM</c:v>
+                  <c:v>Using a VM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1159,7 +1159,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Directry On Machine</c:v>
+                  <c:v>Directly On Machine</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1224,7 +1224,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On Container</c:v>
+                  <c:v>Using a Container</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1289,7 +1289,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>On VM</c:v>
+                  <c:v>Using a VM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3255,15 +3255,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3590,8 +3590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA56488-1A4E-4019-A312-7AB40DC1F38A}">
   <dimension ref="A9:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3604,21 +3604,21 @@
   <sheetData>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>27</v>
@@ -3660,21 +3660,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>2.7</v>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>2.8</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -3716,21 +3716,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>2.77</v>
@@ -3744,7 +3744,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>2.78</v>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>6.37</v>

</xml_diff>

<commit_message>
- added Assignment 2 to README - removed main() from osm.cpp - uploaded graph
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matanel\Documents\University\Year2\SemesterB\67808-OS\Exercises\Ex1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E1F4AF-BA4A-49C3-860B-7125C7652CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF74B571-F339-4576-B2DE-21BBD1F55EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30168" windowHeight="20184" xr2:uid="{C6A71BF6-A859-455F-B82C-36D33C55CA41}"/>
   </bookViews>
@@ -1109,7 +1109,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Runtime</a:t>
+              <a:t>Runtime Comparison</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1174,6 +1174,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-IL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$23:$D$23</c:f>
@@ -1239,6 +1297,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-IL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$23:$D$23</c:f>
@@ -1304,6 +1420,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-IL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$23:$D$23</c:f>
@@ -1346,8 +1520,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1365,6 +1540,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="700" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Function type</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IL" sz="100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1431,6 +1666,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="700"/>
+                  <a:t>Time in nano-seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1476,6 +1766,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14600514741482556"/>
+          <c:y val="0.81646017524767822"/>
+          <c:w val="0.81877313203589464"/>
+          <c:h val="0.11044671049546262"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3254,16 +3554,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>669537</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>93855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438265</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>30781</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3590,8 +3890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA56488-1A4E-4019-A312-7AB40DC1F38A}">
   <dimension ref="A9:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>